<commit_message>
docs: Update sample files with high-quality names (famous people, characters)
</commit_message>
<xml_diff>
--- a/public/samples/sample_data_basic.xlsx
+++ b/public/samples/sample_data_basic.xlsx
@@ -436,7 +436,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="str">
-        <v>강백호</v>
+        <v>정명석</v>
       </c>
       <c r="E2" t="str">
         <v>여</v>
@@ -459,7 +459,7 @@
         <v>2</v>
       </c>
       <c r="D3" t="str">
-        <v>서태웅</v>
+        <v>천송이</v>
       </c>
       <c r="E3" t="str">
         <v>남</v>
@@ -482,7 +482,7 @@
         <v>3</v>
       </c>
       <c r="D4" t="str">
-        <v>채치수</v>
+        <v>김낙수</v>
       </c>
       <c r="E4" t="str">
         <v>남</v>
@@ -505,7 +505,7 @@
         <v>4</v>
       </c>
       <c r="D5" t="str">
-        <v>정대만</v>
+        <v>이상윤</v>
       </c>
       <c r="E5" t="str">
         <v>여</v>
@@ -528,7 +528,7 @@
         <v>5</v>
       </c>
       <c r="D6" t="str">
-        <v>송태섭</v>
+        <v>박연진</v>
       </c>
       <c r="E6" t="str">
         <v>남</v>
@@ -551,7 +551,7 @@
         <v>6</v>
       </c>
       <c r="D7" t="str">
-        <v>권준호</v>
+        <v>박지민</v>
       </c>
       <c r="E7" t="str">
         <v>여</v>
@@ -574,7 +574,7 @@
         <v>7</v>
       </c>
       <c r="D8" t="str">
-        <v>안한수</v>
+        <v>하인성</v>
       </c>
       <c r="E8" t="str">
         <v>여</v>
@@ -597,7 +597,7 @@
         <v>8</v>
       </c>
       <c r="D9" t="str">
-        <v>이한나</v>
+        <v>정준하</v>
       </c>
       <c r="E9" t="str">
         <v>남</v>
@@ -620,7 +620,7 @@
         <v>9</v>
       </c>
       <c r="D10" t="str">
-        <v>채소연</v>
+        <v>계백</v>
       </c>
       <c r="E10" t="str">
         <v>여</v>
@@ -643,7 +643,7 @@
         <v>10</v>
       </c>
       <c r="D11" t="str">
-        <v>윤대협</v>
+        <v>유지민</v>
       </c>
       <c r="E11" t="str">
         <v>여</v>
@@ -666,7 +666,7 @@
         <v>11</v>
       </c>
       <c r="D12" t="str">
-        <v>변덕규</v>
+        <v>양현종</v>
       </c>
       <c r="E12" t="str">
         <v>여</v>
@@ -689,7 +689,7 @@
         <v>12</v>
       </c>
       <c r="D13" t="str">
-        <v>황태산</v>
+        <v>김희철</v>
       </c>
       <c r="E13" t="str">
         <v>남</v>
@@ -712,7 +712,7 @@
         <v>13</v>
       </c>
       <c r="D14" t="str">
-        <v>김수겸</v>
+        <v>이석민</v>
       </c>
       <c r="E14" t="str">
         <v>여</v>
@@ -735,7 +735,7 @@
         <v>14</v>
       </c>
       <c r="D15" t="str">
-        <v>성현준</v>
+        <v>이상순</v>
       </c>
       <c r="E15" t="str">
         <v>남</v>
@@ -758,7 +758,7 @@
         <v>15</v>
       </c>
       <c r="D16" t="str">
-        <v>이정환</v>
+        <v>양세형</v>
       </c>
       <c r="E16" t="str">
         <v>남</v>
@@ -781,7 +781,7 @@
         <v>16</v>
       </c>
       <c r="D17" t="str">
-        <v>전호장</v>
+        <v>서장훈</v>
       </c>
       <c r="E17" t="str">
         <v>여</v>
@@ -804,7 +804,7 @@
         <v>17</v>
       </c>
       <c r="D18" t="str">
-        <v>신준섭</v>
+        <v>한소라</v>
       </c>
       <c r="E18" t="str">
         <v>남</v>
@@ -827,7 +827,7 @@
         <v>18</v>
       </c>
       <c r="D19" t="str">
-        <v>홍익현</v>
+        <v>임꺽정</v>
       </c>
       <c r="E19" t="str">
         <v>남</v>
@@ -850,7 +850,7 @@
         <v>19</v>
       </c>
       <c r="D20" t="str">
-        <v>고민구</v>
+        <v>김구</v>
       </c>
       <c r="E20" t="str">
         <v>남</v>
@@ -873,7 +873,7 @@
         <v>20</v>
       </c>
       <c r="D21" t="str">
-        <v>장권혁</v>
+        <v>강동원</v>
       </c>
       <c r="E21" t="str">
         <v>여</v>
@@ -896,7 +896,7 @@
         <v>21</v>
       </c>
       <c r="D22" t="str">
-        <v>신짱구</v>
+        <v>안산</v>
       </c>
       <c r="E22" t="str">
         <v>여</v>
@@ -919,7 +919,7 @@
         <v>22</v>
       </c>
       <c r="D23" t="str">
-        <v>김철수</v>
+        <v>정우성</v>
       </c>
       <c r="E23" t="str">
         <v>여</v>
@@ -942,7 +942,7 @@
         <v>23</v>
       </c>
       <c r="D24" t="str">
-        <v>한유리</v>
+        <v>전우치</v>
       </c>
       <c r="E24" t="str">
         <v>남</v>
@@ -965,7 +965,7 @@
         <v>24</v>
       </c>
       <c r="D25" t="str">
-        <v>이훈이</v>
+        <v>황광희</v>
       </c>
       <c r="E25" t="str">
         <v>여</v>
@@ -988,7 +988,7 @@
         <v>25</v>
       </c>
       <c r="D26" t="str">
-        <v>나미리</v>
+        <v>김영권</v>
       </c>
       <c r="E26" t="str">
         <v>남</v>
@@ -1011,7 +1011,7 @@
         <v>26</v>
       </c>
       <c r="D27" t="str">
-        <v>채성아</v>
+        <v>이정재</v>
       </c>
       <c r="E27" t="str">
         <v>여</v>
@@ -1034,7 +1034,7 @@
         <v>27</v>
       </c>
       <c r="D28" t="str">
-        <v>노진구</v>
+        <v>고길동</v>
       </c>
       <c r="E28" t="str">
         <v>남</v>
@@ -1057,7 +1057,7 @@
         <v>28</v>
       </c>
       <c r="D29" t="str">
-        <v>신이슬</v>
+        <v>민경훈</v>
       </c>
       <c r="E29" t="str">
         <v>남</v>
@@ -1080,7 +1080,7 @@
         <v>1</v>
       </c>
       <c r="D30" t="str">
-        <v>만퉁퉁</v>
+        <v>강호동</v>
       </c>
       <c r="E30" t="str">
         <v>여</v>
@@ -1103,7 +1103,7 @@
         <v>2</v>
       </c>
       <c r="D31" t="str">
-        <v>왕비실</v>
+        <v>이마크</v>
       </c>
       <c r="E31" t="str">
         <v>남</v>
@@ -1126,7 +1126,7 @@
         <v>3</v>
       </c>
       <c r="D32" t="str">
-        <v>박영민</v>
+        <v>유시진</v>
       </c>
       <c r="E32" t="str">
         <v>여</v>
@@ -1149,7 +1149,7 @@
         <v>4</v>
       </c>
       <c r="D33" t="str">
-        <v>남도일</v>
+        <v>김준완</v>
       </c>
       <c r="E33" t="str">
         <v>남</v>
@@ -1172,7 +1172,7 @@
         <v>5</v>
       </c>
       <c r="D34" t="str">
-        <v>유미란</v>
+        <v>서대영</v>
       </c>
       <c r="E34" t="str">
         <v>남</v>
@@ -1195,7 +1195,7 @@
         <v>6</v>
       </c>
       <c r="D35" t="str">
-        <v>유명한</v>
+        <v>이혜인</v>
       </c>
       <c r="E35" t="str">
         <v>남</v>
@@ -1218,7 +1218,7 @@
         <v>7</v>
       </c>
       <c r="D36" t="str">
-        <v>홍장미</v>
+        <v>변백현</v>
       </c>
       <c r="E36" t="str">
         <v>여</v>
@@ -1241,7 +1241,7 @@
         <v>8</v>
       </c>
       <c r="D37" t="str">
-        <v>고뭉치</v>
+        <v>표지훈</v>
       </c>
       <c r="E37" t="str">
         <v>여</v>
@@ -1264,7 +1264,7 @@
         <v>9</v>
       </c>
       <c r="D38" t="str">
-        <v>박세모</v>
+        <v>서영호</v>
       </c>
       <c r="E38" t="str">
         <v>남</v>
@@ -1287,7 +1287,7 @@
         <v>10</v>
       </c>
       <c r="D39" t="str">
-        <v>한아름</v>
+        <v>유미란</v>
       </c>
       <c r="E39" t="str">
         <v>여</v>
@@ -1310,7 +1310,7 @@
         <v>11</v>
       </c>
       <c r="D40" t="str">
-        <v>하인성</v>
+        <v>송태섭</v>
       </c>
       <c r="E40" t="str">
         <v>여</v>
@@ -1333,7 +1333,7 @@
         <v>12</v>
       </c>
       <c r="D41" t="str">
-        <v>서가영</v>
+        <v>채치수</v>
       </c>
       <c r="E41" t="str">
         <v>여</v>
@@ -1356,7 +1356,7 @@
         <v>13</v>
       </c>
       <c r="D42" t="str">
-        <v>이상윤</v>
+        <v>최혜정</v>
       </c>
       <c r="E42" t="str">
         <v>여</v>
@@ -1379,7 +1379,7 @@
         <v>14</v>
       </c>
       <c r="D43" t="str">
-        <v>안기준</v>
+        <v>김수겸</v>
       </c>
       <c r="E43" t="str">
         <v>남</v>
@@ -1402,7 +1402,7 @@
         <v>15</v>
       </c>
       <c r="D44" t="str">
-        <v>정보라</v>
+        <v>공유</v>
       </c>
       <c r="E44" t="str">
         <v>남</v>
@@ -1425,7 +1425,7 @@
         <v>16</v>
       </c>
       <c r="D45" t="str">
-        <v>하쿠나</v>
+        <v>신태일</v>
       </c>
       <c r="E45" t="str">
         <v>남</v>
@@ -1448,7 +1448,7 @@
         <v>17</v>
       </c>
       <c r="D46" t="str">
-        <v>치히로</v>
+        <v>이재하</v>
       </c>
       <c r="E46" t="str">
         <v>남</v>
@@ -1471,7 +1471,7 @@
         <v>18</v>
       </c>
       <c r="D47" t="str">
-        <v>소스케</v>
+        <v>윤정한</v>
       </c>
       <c r="E47" t="str">
         <v>남</v>
@@ -1494,7 +1494,7 @@
         <v>19</v>
       </c>
       <c r="D48" t="str">
-        <v>토토로</v>
+        <v>홍예지</v>
       </c>
       <c r="E48" t="str">
         <v>남</v>
@@ -1517,7 +1517,7 @@
         <v>20</v>
       </c>
       <c r="D49" t="str">
-        <v>탄지로</v>
+        <v>구하리</v>
       </c>
       <c r="E49" t="str">
         <v>남</v>
@@ -1540,7 +1540,7 @@
         <v>21</v>
       </c>
       <c r="D50" t="str">
-        <v>네즈코</v>
+        <v>양세찬</v>
       </c>
       <c r="E50" t="str">
         <v>남</v>
@@ -1563,7 +1563,7 @@
         <v>22</v>
       </c>
       <c r="D51" t="str">
-        <v>젠이츠</v>
+        <v>박흥부</v>
       </c>
       <c r="E51" t="str">
         <v>남</v>
@@ -1586,7 +1586,7 @@
         <v>23</v>
       </c>
       <c r="D52" t="str">
-        <v>이노스</v>
+        <v>김지원</v>
       </c>
       <c r="E52" t="str">
         <v>여</v>
@@ -1609,7 +1609,7 @@
         <v>24</v>
       </c>
       <c r="D53" t="str">
-        <v>기유</v>
+        <v>추신수</v>
       </c>
       <c r="E53" t="str">
         <v>여</v>
@@ -1632,7 +1632,7 @@
         <v>25</v>
       </c>
       <c r="D54" t="str">
-        <v>시노부</v>
+        <v>나재민</v>
       </c>
       <c r="E54" t="str">
         <v>여</v>
@@ -1655,7 +1655,7 @@
         <v>26</v>
       </c>
       <c r="D55" t="str">
-        <v>렌고쿠</v>
+        <v>염기정</v>
       </c>
       <c r="E55" t="str">
         <v>남</v>
@@ -1678,7 +1678,7 @@
         <v>27</v>
       </c>
       <c r="D56" t="str">
-        <v>무이치</v>
+        <v>동그라</v>
       </c>
       <c r="E56" t="str">
         <v>여</v>
@@ -1701,7 +1701,7 @@
         <v>1</v>
       </c>
       <c r="D57" t="str">
-        <v>사네미</v>
+        <v>현빈</v>
       </c>
       <c r="E57" t="str">
         <v>남</v>
@@ -1724,7 +1724,7 @@
         <v>2</v>
       </c>
       <c r="D58" t="str">
-        <v>홍길동</v>
+        <v>맹사성</v>
       </c>
       <c r="E58" t="str">
         <v>여</v>
@@ -1747,7 +1747,7 @@
         <v>3</v>
       </c>
       <c r="D59" t="str">
-        <v>성춘향</v>
+        <v>성기훈</v>
       </c>
       <c r="E59" t="str">
         <v>남</v>
@@ -1770,7 +1770,7 @@
         <v>4</v>
       </c>
       <c r="D60" t="str">
-        <v>이몽룡</v>
+        <v>김태희</v>
       </c>
       <c r="E60" t="str">
         <v>남</v>
@@ -1793,7 +1793,7 @@
         <v>5</v>
       </c>
       <c r="D61" t="str">
-        <v>변학도</v>
+        <v>이정후</v>
       </c>
       <c r="E61" t="str">
         <v>여</v>
@@ -1816,7 +1816,7 @@
         <v>6</v>
       </c>
       <c r="D62" t="str">
-        <v>심청이</v>
+        <v>권순영</v>
       </c>
       <c r="E62" t="str">
         <v>남</v>
@@ -1839,7 +1839,7 @@
         <v>7</v>
       </c>
       <c r="D63" t="str">
-        <v>박흥부</v>
+        <v>유명한</v>
       </c>
       <c r="E63" t="str">
         <v>남</v>
@@ -1862,7 +1862,7 @@
         <v>8</v>
       </c>
       <c r="D64" t="str">
-        <v>박놀부</v>
+        <v>이상우</v>
       </c>
       <c r="E64" t="str">
         <v>여</v>
@@ -1885,7 +1885,7 @@
         <v>9</v>
       </c>
       <c r="D65" t="str">
-        <v>임꺽정</v>
+        <v>정석</v>
       </c>
       <c r="E65" t="str">
         <v>남</v>
@@ -1908,7 +1908,7 @@
         <v>10</v>
       </c>
       <c r="D66" t="str">
-        <v>장장화</v>
+        <v>김도영</v>
       </c>
       <c r="E66" t="str">
         <v>여</v>
@@ -1931,7 +1931,7 @@
         <v>11</v>
       </c>
       <c r="D67" t="str">
-        <v>장홍련</v>
+        <v>김수현</v>
       </c>
       <c r="E67" t="str">
         <v>여</v>
@@ -1954,7 +1954,7 @@
         <v>12</v>
       </c>
       <c r="D68" t="str">
-        <v>김선달</v>
+        <v>이정환</v>
       </c>
       <c r="E68" t="str">
         <v>여</v>
@@ -1977,7 +1977,7 @@
         <v>13</v>
       </c>
       <c r="D69" t="str">
-        <v>황진이</v>
+        <v>황희찬</v>
       </c>
       <c r="E69" t="str">
         <v>남</v>
@@ -2000,7 +2000,7 @@
         <v>14</v>
       </c>
       <c r="D70" t="str">
-        <v>논개</v>
+        <v>김고은</v>
       </c>
       <c r="E70" t="str">
         <v>남</v>
@@ -2023,7 +2023,7 @@
         <v>15</v>
       </c>
       <c r="D71" t="str">
-        <v>신사임</v>
+        <v>맹구</v>
       </c>
       <c r="E71" t="str">
         <v>남</v>
@@ -2046,7 +2046,7 @@
         <v>16</v>
       </c>
       <c r="D72" t="str">
-        <v>이순신</v>
+        <v>강해린</v>
       </c>
       <c r="E72" t="str">
         <v>여</v>
@@ -2069,7 +2069,7 @@
         <v>17</v>
       </c>
       <c r="D73" t="str">
-        <v>세종대</v>
+        <v>유관순</v>
       </c>
       <c r="E73" t="str">
         <v>남</v>
@@ -2092,7 +2092,7 @@
         <v>18</v>
       </c>
       <c r="D74" t="str">
-        <v>장영실</v>
+        <v>한석봉</v>
       </c>
       <c r="E74" t="str">
         <v>남</v>
@@ -2115,7 +2115,7 @@
         <v>19</v>
       </c>
       <c r="D75" t="str">
-        <v>정약용</v>
+        <v>안영수</v>
       </c>
       <c r="E75" t="str">
         <v>여</v>
@@ -2138,7 +2138,7 @@
         <v>20</v>
       </c>
       <c r="D76" t="str">
-        <v>김정호</v>
+        <v>박찬호</v>
       </c>
       <c r="E76" t="str">
         <v>여</v>
@@ -2161,7 +2161,7 @@
         <v>21</v>
       </c>
       <c r="D77" t="str">
-        <v>한석봉</v>
+        <v>박지원</v>
       </c>
       <c r="E77" t="str">
         <v>남</v>
@@ -2184,7 +2184,7 @@
         <v>22</v>
       </c>
       <c r="D78" t="str">
-        <v>김구</v>
+        <v>황선우</v>
       </c>
       <c r="E78" t="str">
         <v>남</v>
@@ -2207,7 +2207,7 @@
         <v>23</v>
       </c>
       <c r="D79" t="str">
-        <v>안중근</v>
+        <v>박보영</v>
       </c>
       <c r="E79" t="str">
         <v>여</v>
@@ -2230,7 +2230,7 @@
         <v>24</v>
       </c>
       <c r="D80" t="str">
-        <v>윤봉길</v>
+        <v>홍길동</v>
       </c>
       <c r="E80" t="str">
         <v>여</v>
@@ -2253,7 +2253,7 @@
         <v>25</v>
       </c>
       <c r="D81" t="str">
-        <v>유관순</v>
+        <v>송민호</v>
       </c>
       <c r="E81" t="str">
         <v>여</v>
@@ -2276,7 +2276,7 @@
         <v>26</v>
       </c>
       <c r="D82" t="str">
-        <v>유재석</v>
+        <v>서태웅</v>
       </c>
       <c r="E82" t="str">
         <v>여</v>
@@ -2299,7 +2299,7 @@
         <v>27</v>
       </c>
       <c r="D83" t="str">
-        <v>박명수</v>
+        <v>안창호</v>
       </c>
       <c r="E83" t="str">
         <v>여</v>
@@ -2322,7 +2322,7 @@
         <v>28</v>
       </c>
       <c r="D84" t="str">
-        <v>정준하</v>
+        <v>홍장미</v>
       </c>
       <c r="E84" t="str">
         <v>남</v>
@@ -2345,7 +2345,7 @@
         <v>1</v>
       </c>
       <c r="D85" t="str">
-        <v>하동훈</v>
+        <v>봉미선</v>
       </c>
       <c r="E85" t="str">
         <v>여</v>
@@ -2368,7 +2368,7 @@
         <v>2</v>
       </c>
       <c r="D86" t="str">
-        <v>노홍철</v>
+        <v>이광수</v>
       </c>
       <c r="E86" t="str">
         <v>남</v>
@@ -2391,7 +2391,7 @@
         <v>3</v>
       </c>
       <c r="D87" t="str">
-        <v>정형돈</v>
+        <v>신짱아</v>
       </c>
       <c r="E87" t="str">
         <v>남</v>
@@ -2414,7 +2414,7 @@
         <v>4</v>
       </c>
       <c r="D88" t="str">
-        <v>길성준</v>
+        <v>홍은채</v>
       </c>
       <c r="E88" t="str">
         <v>남</v>
@@ -2437,7 +2437,7 @@
         <v>5</v>
       </c>
       <c r="D89" t="str">
-        <v>황광희</v>
+        <v>강새벽</v>
       </c>
       <c r="E89" t="str">
         <v>남</v>
@@ -2460,7 +2460,7 @@
         <v>6</v>
       </c>
       <c r="D90" t="str">
-        <v>조세호</v>
+        <v>정호석</v>
       </c>
       <c r="E90" t="str">
         <v>남</v>
@@ -2483,7 +2483,7 @@
         <v>7</v>
       </c>
       <c r="D91" t="str">
-        <v>양세형</v>
+        <v>안한수</v>
       </c>
       <c r="E91" t="str">
         <v>여</v>
@@ -2506,7 +2506,7 @@
         <v>8</v>
       </c>
       <c r="D92" t="str">
-        <v>이광수</v>
+        <v>황준호</v>
       </c>
       <c r="E92" t="str">
         <v>여</v>
@@ -2529,7 +2529,7 @@
         <v>9</v>
       </c>
       <c r="D93" t="str">
-        <v>김종국</v>
+        <v>뺑덕이</v>
       </c>
       <c r="E93" t="str">
         <v>여</v>
@@ -2552,7 +2552,7 @@
         <v>10</v>
       </c>
       <c r="D94" t="str">
-        <v>송지효</v>
+        <v>소지섭</v>
       </c>
       <c r="E94" t="str">
         <v>남</v>
@@ -2575,7 +2575,7 @@
         <v>11</v>
       </c>
       <c r="D95" t="str">
-        <v>강호동</v>
+        <v>최동오</v>
       </c>
       <c r="E95" t="str">
         <v>여</v>
@@ -2598,7 +2598,7 @@
         <v>12</v>
       </c>
       <c r="D96" t="str">
-        <v>이수근</v>
+        <v>김민규</v>
       </c>
       <c r="E96" t="str">
         <v>남</v>
@@ -2621,7 +2621,7 @@
         <v>13</v>
       </c>
       <c r="D97" t="str">
-        <v>은지원</v>
+        <v>허윤진</v>
       </c>
       <c r="E97" t="str">
         <v>여</v>
@@ -2644,7 +2644,7 @@
         <v>14</v>
       </c>
       <c r="D98" t="str">
-        <v>안재현</v>
+        <v>김진수</v>
       </c>
       <c r="E98" t="str">
         <v>남</v>
@@ -2667,7 +2667,7 @@
         <v>15</v>
       </c>
       <c r="D99" t="str">
-        <v>조규현</v>
+        <v>김동식</v>
       </c>
       <c r="E99" t="str">
         <v>여</v>
@@ -2690,7 +2690,7 @@
         <v>16</v>
       </c>
       <c r="D100" t="str">
-        <v>송민호</v>
+        <v>희동이</v>
       </c>
       <c r="E100" t="str">
         <v>여</v>
@@ -2713,7 +2713,7 @@
         <v>17</v>
       </c>
       <c r="D101" t="str">
-        <v>표지훈</v>
+        <v>성선우</v>
       </c>
       <c r="E101" t="str">
         <v>남</v>
@@ -2736,7 +2736,7 @@
         <v>18</v>
       </c>
       <c r="D102" t="str">
-        <v>김희철</v>
+        <v>김현우</v>
       </c>
       <c r="E102" t="str">
         <v>여</v>
@@ -2759,7 +2759,7 @@
         <v>19</v>
       </c>
       <c r="D103" t="str">
-        <v>민경훈</v>
+        <v>심봉사</v>
       </c>
       <c r="E103" t="str">
         <v>남</v>
@@ -2782,7 +2782,7 @@
         <v>20</v>
       </c>
       <c r="D104" t="str">
-        <v>서장훈</v>
+        <v>남훈</v>
       </c>
       <c r="E104" t="str">
         <v>남</v>
@@ -2805,7 +2805,7 @@
         <v>21</v>
       </c>
       <c r="D105" t="str">
-        <v>이상민</v>
+        <v>유명호</v>
       </c>
       <c r="E105" t="str">
         <v>여</v>
@@ -2828,7 +2828,7 @@
         <v>22</v>
       </c>
       <c r="D106" t="str">
-        <v>아이유</v>
+        <v>김영철</v>
       </c>
       <c r="E106" t="str">
         <v>여</v>
@@ -2851,7 +2851,7 @@
         <v>23</v>
       </c>
       <c r="D107" t="str">
-        <v>박효신</v>
+        <v>방정환</v>
       </c>
       <c r="E107" t="str">
         <v>남</v>
@@ -2874,7 +2874,7 @@
         <v>24</v>
       </c>
       <c r="D108" t="str">
-        <v>나얼</v>
+        <v>성춘향</v>
       </c>
       <c r="E108" t="str">
         <v>남</v>
@@ -2897,7 +2897,7 @@
         <v>25</v>
       </c>
       <c r="D109" t="str">
-        <v>김범수</v>
+        <v>강동준</v>
       </c>
       <c r="E109" t="str">
         <v>남</v>
@@ -2920,7 +2920,7 @@
         <v>26</v>
       </c>
       <c r="D110" t="str">
-        <v>이선희</v>
+        <v>황인범</v>
       </c>
       <c r="E110" t="str">
         <v>남</v>
@@ -2943,7 +2943,7 @@
         <v>27</v>
       </c>
       <c r="D111" t="str">
-        <v>임재범</v>
+        <v>권문아</v>
       </c>
       <c r="E111" t="str">
         <v>여</v>
@@ -2966,7 +2966,7 @@
         <v>1</v>
       </c>
       <c r="D112" t="str">
-        <v>박정현</v>
+        <v>이현서</v>
       </c>
       <c r="E112" t="str">
         <v>남</v>
@@ -2989,7 +2989,7 @@
         <v>2</v>
       </c>
       <c r="D113" t="str">
-        <v>이승기</v>
+        <v>도진우</v>
       </c>
       <c r="E113" t="str">
         <v>남</v>
@@ -3012,7 +3012,7 @@
         <v>3</v>
       </c>
       <c r="D114" t="str">
-        <v>차은우</v>
+        <v>이영표</v>
       </c>
       <c r="E114" t="str">
         <v>여</v>
@@ -3035,7 +3035,7 @@
         <v>4</v>
       </c>
       <c r="D115" t="str">
-        <v>김태리</v>
+        <v>오세훈</v>
       </c>
       <c r="E115" t="str">
         <v>여</v>
@@ -3058,7 +3058,7 @@
         <v>5</v>
       </c>
       <c r="D116" t="str">
-        <v>한소희</v>
+        <v>서가영</v>
       </c>
       <c r="E116" t="str">
         <v>남</v>
@@ -3081,7 +3081,7 @@
         <v>6</v>
       </c>
       <c r="D117" t="str">
-        <v>송강</v>
+        <v>오일남</v>
       </c>
       <c r="E117" t="str">
         <v>여</v>
@@ -3104,7 +3104,7 @@
         <v>7</v>
       </c>
       <c r="D118" t="str">
-        <v>박보영</v>
+        <v>추민하</v>
       </c>
       <c r="E118" t="str">
         <v>여</v>
@@ -3127,7 +3127,7 @@
         <v>8</v>
       </c>
       <c r="D119" t="str">
-        <v>조정석</v>
+        <v>최강림</v>
       </c>
       <c r="E119" t="str">
         <v>여</v>
@@ -3150,7 +3150,7 @@
         <v>9</v>
       </c>
       <c r="D120" t="str">
-        <v>전미도</v>
+        <v>김정호</v>
       </c>
       <c r="E120" t="str">
         <v>남</v>
@@ -3173,7 +3173,7 @@
         <v>10</v>
       </c>
       <c r="D121" t="str">
-        <v>유연석</v>
+        <v>손연재</v>
       </c>
       <c r="E121" t="str">
         <v>여</v>
@@ -3196,7 +3196,7 @@
         <v>11</v>
       </c>
       <c r="D122" t="str">
-        <v>정경호</v>
+        <v>하동훈</v>
       </c>
       <c r="E122" t="str">
         <v>여</v>
@@ -3219,7 +3219,7 @@
         <v>12</v>
       </c>
       <c r="D123" t="str">
-        <v>김대명</v>
+        <v>이찬</v>
       </c>
       <c r="E123" t="str">
         <v>남</v>
@@ -3242,7 +3242,7 @@
         <v>13</v>
       </c>
       <c r="D124" t="str">
-        <v>손흥민</v>
+        <v>류현진</v>
       </c>
       <c r="E124" t="str">
         <v>여</v>
@@ -3265,7 +3265,7 @@
         <v>14</v>
       </c>
       <c r="D125" t="str">
-        <v>이강인</v>
+        <v>김정봉</v>
       </c>
       <c r="E125" t="str">
         <v>남</v>
@@ -3288,7 +3288,7 @@
         <v>15</v>
       </c>
       <c r="D126" t="str">
-        <v>김민재</v>
+        <v>전지현</v>
       </c>
       <c r="E126" t="str">
         <v>여</v>
@@ -3311,7 +3311,7 @@
         <v>16</v>
       </c>
       <c r="D127" t="str">
-        <v>황희찬</v>
+        <v>이사라</v>
       </c>
       <c r="E127" t="str">
         <v>남</v>
@@ -3334,7 +3334,7 @@
         <v>17</v>
       </c>
       <c r="D128" t="str">
-        <v>조규성</v>
+        <v>문동은</v>
       </c>
       <c r="E128" t="str">
         <v>남</v>
@@ -3357,7 +3357,7 @@
         <v>18</v>
       </c>
       <c r="D129" t="str">
-        <v>황인범</v>
+        <v>강백호</v>
       </c>
       <c r="E129" t="str">
         <v>여</v>
@@ -3380,7 +3380,7 @@
         <v>19</v>
       </c>
       <c r="D130" t="str">
-        <v>이승우</v>
+        <v>조인성</v>
       </c>
       <c r="E130" t="str">
         <v>남</v>
@@ -3403,7 +3403,7 @@
         <v>20</v>
       </c>
       <c r="D131" t="str">
-        <v>박지성</v>
+        <v>이상민</v>
       </c>
       <c r="E131" t="str">
         <v>여</v>
@@ -3426,7 +3426,7 @@
         <v>21</v>
       </c>
       <c r="D132" t="str">
-        <v>이영표</v>
+        <v>강감찬</v>
       </c>
       <c r="E132" t="str">
         <v>여</v>
@@ -3449,7 +3449,7 @@
         <v>22</v>
       </c>
       <c r="D133" t="str">
-        <v>안정환</v>
+        <v>리온</v>
       </c>
       <c r="E133" t="str">
         <v>여</v>
@@ -3472,7 +3472,7 @@
         <v>23</v>
       </c>
       <c r="D134" t="str">
-        <v>차두리</v>
+        <v>김하성</v>
       </c>
       <c r="E134" t="str">
         <v>여</v>
@@ -3495,7 +3495,7 @@
         <v>24</v>
       </c>
       <c r="D135" t="str">
-        <v>류현진</v>
+        <v>유덕화</v>
       </c>
       <c r="E135" t="str">
         <v>남</v>
@@ -3518,7 +3518,7 @@
         <v>25</v>
       </c>
       <c r="D136" t="str">
-        <v>추신수</v>
+        <v>노홍철</v>
       </c>
       <c r="E136" t="str">
         <v>남</v>
@@ -3541,7 +3541,7 @@
         <v>26</v>
       </c>
       <c r="D137" t="str">
-        <v>이정후</v>
+        <v>이승엽</v>
       </c>
       <c r="E137" t="str">
         <v>남</v>
@@ -3564,7 +3564,7 @@
         <v>27</v>
       </c>
       <c r="D138" t="str">
-        <v>김연아</v>
+        <v>장미란</v>
       </c>
       <c r="E138" t="str">
         <v>남</v>
@@ -3587,7 +3587,7 @@
         <v>28</v>
       </c>
       <c r="D139" t="str">
-        <v>손연재</v>
+        <v>설경구</v>
       </c>
       <c r="E139" t="str">
         <v>남</v>
@@ -3610,7 +3610,7 @@
         <v>1</v>
       </c>
       <c r="D140" t="str">
-        <v>장미란</v>
+        <v>서명호</v>
       </c>
       <c r="E140" t="str">
         <v>여</v>
@@ -3633,7 +3633,7 @@
         <v>2</v>
       </c>
       <c r="D141" t="str">
-        <v>박태환</v>
+        <v>박명수</v>
       </c>
       <c r="E141" t="str">
         <v>남</v>
@@ -3656,7 +3656,7 @@
         <v>3</v>
       </c>
       <c r="D142" t="str">
-        <v>해리포</v>
+        <v>김홍도</v>
       </c>
       <c r="E142" t="str">
         <v>남</v>
@@ -3679,7 +3679,7 @@
         <v>4</v>
       </c>
       <c r="D143" t="str">
-        <v>론위즐</v>
+        <v>권민우</v>
       </c>
       <c r="E143" t="str">
         <v>남</v>
@@ -3702,7 +3702,7 @@
         <v>5</v>
       </c>
       <c r="D144" t="str">
-        <v>헤르미</v>
+        <v>박병호</v>
       </c>
       <c r="E144" t="str">
         <v>남</v>
@@ -3725,7 +3725,7 @@
         <v>6</v>
       </c>
       <c r="D145" t="str">
-        <v>말포이</v>
+        <v>한아름</v>
       </c>
       <c r="E145" t="str">
         <v>남</v>
@@ -3748,7 +3748,7 @@
         <v>7</v>
       </c>
       <c r="D146" t="str">
-        <v>해그리</v>
+        <v>최한솔</v>
       </c>
       <c r="E146" t="str">
         <v>남</v>
@@ -3771,7 +3771,7 @@
         <v>8</v>
       </c>
       <c r="D147" t="str">
-        <v>덤블도</v>
+        <v>장장화</v>
       </c>
       <c r="E147" t="str">
         <v>여</v>
@@ -3794,7 +3794,7 @@
         <v>9</v>
       </c>
       <c r="D148" t="str">
-        <v>스네이</v>
+        <v>이운재</v>
       </c>
       <c r="E148" t="str">
         <v>여</v>
@@ -3817,7 +3817,7 @@
         <v>10</v>
       </c>
       <c r="D149" t="str">
-        <v>토니박</v>
+        <v>이태용</v>
       </c>
       <c r="E149" t="str">
         <v>남</v>
@@ -3840,7 +3840,7 @@
         <v>11</v>
       </c>
       <c r="D150" t="str">
-        <v>스티브</v>
+        <v>저승이</v>
       </c>
       <c r="E150" t="str">
         <v>여</v>
@@ -3863,7 +3863,7 @@
         <v>12</v>
       </c>
       <c r="D151" t="str">
-        <v>토르김</v>
+        <v>이명헌</v>
       </c>
       <c r="E151" t="str">
         <v>남</v>
@@ -3886,7 +3886,7 @@
         <v>13</v>
       </c>
       <c r="D152" t="str">
-        <v>배너박</v>
+        <v>정재현</v>
       </c>
       <c r="E152" t="str">
         <v>여</v>
@@ -3909,7 +3909,7 @@
         <v>14</v>
       </c>
       <c r="D153" t="str">
-        <v>나타샤</v>
+        <v>성보라</v>
       </c>
       <c r="E153" t="str">
         <v>남</v>
@@ -3932,7 +3932,7 @@
         <v>15</v>
       </c>
       <c r="D154" t="str">
-        <v>바튼조</v>
+        <v>한효주</v>
       </c>
       <c r="E154" t="str">
         <v>남</v>
@@ -3955,7 +3955,7 @@
         <v>16</v>
       </c>
       <c r="D155" t="str">
-        <v>피터팬</v>
+        <v>설기현</v>
       </c>
       <c r="E155" t="str">
         <v>여</v>
@@ -3978,7 +3978,7 @@
         <v>17</v>
       </c>
       <c r="D156" t="str">
-        <v>김민수</v>
+        <v>손명오</v>
       </c>
       <c r="E156" t="str">
         <v>여</v>
@@ -4001,7 +4001,7 @@
         <v>18</v>
       </c>
       <c r="D157" t="str">
-        <v>이서준</v>
+        <v>도재학</v>
       </c>
       <c r="E157" t="str">
         <v>여</v>
@@ -4024,7 +4024,7 @@
         <v>19</v>
       </c>
       <c r="D158" t="str">
-        <v>박지훈</v>
+        <v>송중기</v>
       </c>
       <c r="E158" t="str">
         <v>남</v>
@@ -4047,7 +4047,7 @@
         <v>20</v>
       </c>
       <c r="D159" t="str">
-        <v>최예준</v>
+        <v>하정우</v>
       </c>
       <c r="E159" t="str">
         <v>남</v>
@@ -4070,7 +4070,7 @@
         <v>21</v>
       </c>
       <c r="D160" t="str">
-        <v>정현우</v>
+        <v>공효진</v>
       </c>
       <c r="E160" t="str">
         <v>여</v>
@@ -4093,7 +4093,7 @@
         <v>22</v>
       </c>
       <c r="D161" t="str">
-        <v>강시우</v>
+        <v>최진철</v>
       </c>
       <c r="E161" t="str">
         <v>여</v>
@@ -4116,7 +4116,7 @@
         <v>23</v>
       </c>
       <c r="D162" t="str">
-        <v>조도현</v>
+        <v>김대남</v>
       </c>
       <c r="E162" t="str">
         <v>남</v>
@@ -4139,7 +4139,7 @@
         <v>24</v>
       </c>
       <c r="D163" t="str">
-        <v>윤건우</v>
+        <v>신유빈</v>
       </c>
       <c r="E163" t="str">
         <v>여</v>
@@ -4162,7 +4162,7 @@
         <v>25</v>
       </c>
       <c r="D164" t="str">
-        <v>장준우</v>
+        <v>신형만</v>
       </c>
       <c r="E164" t="str">
         <v>남</v>
@@ -4185,7 +4185,7 @@
         <v>26</v>
       </c>
       <c r="D165" t="str">
-        <v>임지호</v>
+        <v>한유리</v>
       </c>
       <c r="E165" t="str">
         <v>남</v>
@@ -4208,7 +4208,7 @@
         <v>27</v>
       </c>
       <c r="D166" t="str">
-        <v>한서윤</v>
+        <v>김가을</v>
       </c>
       <c r="E166" t="str">
         <v>여</v>
@@ -4231,7 +4231,7 @@
         <v>1</v>
       </c>
       <c r="D167" t="str">
-        <v>오서연</v>
+        <v>유재석</v>
       </c>
       <c r="E167" t="str">
         <v>남</v>
@@ -4254,7 +4254,7 @@
         <v>2</v>
       </c>
       <c r="D168" t="str">
-        <v>서지우</v>
+        <v>팥쥐</v>
       </c>
       <c r="E168" t="str">
         <v>여</v>
@@ -4277,7 +4277,7 @@
         <v>3</v>
       </c>
       <c r="D169" t="str">
-        <v>신하은</v>
+        <v>서희</v>
       </c>
       <c r="E169" t="str">
         <v>여</v>
@@ -4300,7 +4300,7 @@
         <v>4</v>
       </c>
       <c r="D170" t="str">
-        <v>권도은</v>
+        <v>안재현</v>
       </c>
       <c r="E170" t="str">
         <v>남</v>
@@ -4323,7 +4323,7 @@
         <v>5</v>
       </c>
       <c r="D171" t="str">
-        <v>황수아</v>
+        <v>김채원</v>
       </c>
       <c r="E171" t="str">
         <v>남</v>
@@ -4346,7 +4346,7 @@
         <v>6</v>
       </c>
       <c r="D172" t="str">
-        <v>안지아</v>
+        <v>주여정</v>
       </c>
       <c r="E172" t="str">
         <v>남</v>
@@ -4369,7 +4369,7 @@
         <v>7</v>
       </c>
       <c r="D173" t="str">
-        <v>송서현</v>
+        <v>세종대</v>
       </c>
       <c r="E173" t="str">
         <v>여</v>
@@ -4392,7 +4392,7 @@
         <v>8</v>
       </c>
       <c r="D174" t="str">
-        <v>전하윤</v>
+        <v>조규현</v>
       </c>
       <c r="E174" t="str">
         <v>여</v>
@@ -4415,7 +4415,7 @@
         <v>9</v>
       </c>
       <c r="D175" t="str">
-        <v>홍민서</v>
+        <v>이병헌</v>
       </c>
       <c r="E175" t="str">
         <v>남</v>
@@ -4438,7 +4438,7 @@
         <v>10</v>
       </c>
       <c r="D176" t="str">
-        <v>김서준</v>
+        <v>전호장</v>
       </c>
       <c r="E176" t="str">
         <v>여</v>
@@ -4461,7 +4461,7 @@
         <v>11</v>
       </c>
       <c r="D177" t="str">
-        <v>이도현</v>
+        <v>도우너</v>
       </c>
       <c r="E177" t="str">
         <v>여</v>
@@ -4484,7 +4484,7 @@
         <v>12</v>
       </c>
       <c r="D178" t="str">
-        <v>박하준</v>
+        <v>윤대협</v>
       </c>
       <c r="E178" t="str">
         <v>여</v>
@@ -4507,7 +4507,7 @@
         <v>13</v>
       </c>
       <c r="D179" t="str">
-        <v>최은우</v>
+        <v>신지수</v>
       </c>
       <c r="E179" t="str">
         <v>여</v>
@@ -4530,7 +4530,7 @@
         <v>14</v>
       </c>
       <c r="D180" t="str">
-        <v>정시우</v>
+        <v>유세미</v>
       </c>
       <c r="E180" t="str">
         <v>남</v>
@@ -4553,7 +4553,7 @@
         <v>15</v>
       </c>
       <c r="D181" t="str">
-        <v>강지호</v>
+        <v>홍지수</v>
       </c>
       <c r="E181" t="str">
         <v>여</v>
@@ -4576,7 +4576,7 @@
         <v>16</v>
       </c>
       <c r="D182" t="str">
-        <v>조예준</v>
+        <v>안유진</v>
       </c>
       <c r="E182" t="str">
         <v>여</v>
@@ -4599,7 +4599,7 @@
         <v>17</v>
       </c>
       <c r="D183" t="str">
-        <v>윤민준</v>
+        <v>전재준</v>
       </c>
       <c r="E183" t="str">
         <v>남</v>
@@ -4622,7 +4622,7 @@
         <v>18</v>
       </c>
       <c r="D184" t="str">
-        <v>장유준</v>
+        <v>정성구</v>
       </c>
       <c r="E184" t="str">
         <v>남</v>
@@ -4645,7 +4645,7 @@
         <v>19</v>
       </c>
       <c r="D185" t="str">
-        <v>임주원</v>
+        <v>신짱구</v>
       </c>
       <c r="E185" t="str">
         <v>여</v>
@@ -4668,7 +4668,7 @@
         <v>20</v>
       </c>
       <c r="D186" t="str">
-        <v>한이안</v>
+        <v>유체리</v>
       </c>
       <c r="E186" t="str">
         <v>남</v>
@@ -4691,7 +4691,7 @@
         <v>21</v>
       </c>
       <c r="D187" t="str">
-        <v>오준우</v>
+        <v>김유신</v>
       </c>
       <c r="E187" t="str">
         <v>여</v>
@@ -4714,7 +4714,7 @@
         <v>22</v>
       </c>
       <c r="D188" t="str">
-        <v>서건우</v>
+        <v>마이콜</v>
       </c>
       <c r="E188" t="str">
         <v>남</v>
@@ -4737,7 +4737,7 @@
         <v>23</v>
       </c>
       <c r="D189" t="str">
-        <v>신로운</v>
+        <v>변덕규</v>
       </c>
       <c r="E189" t="str">
         <v>여</v>
@@ -4760,7 +4760,7 @@
         <v>24</v>
       </c>
       <c r="D190" t="str">
-        <v>권우주</v>
+        <v>나미리</v>
       </c>
       <c r="E190" t="str">
         <v>남</v>
@@ -4783,7 +4783,7 @@
         <v>25</v>
       </c>
       <c r="D191" t="str">
-        <v>황선우</v>
+        <v>이미나</v>
       </c>
       <c r="E191" t="str">
         <v>여</v>
@@ -4806,7 +4806,7 @@
         <v>26</v>
       </c>
       <c r="D192" t="str">
-        <v>안서진</v>
+        <v>박지성</v>
       </c>
       <c r="E192" t="str">
         <v>남</v>
@@ -4829,7 +4829,7 @@
         <v>27</v>
       </c>
       <c r="D193" t="str">
-        <v>송연우</v>
+        <v>최수연</v>
       </c>
       <c r="E193" t="str">
         <v>남</v>
@@ -4852,7 +4852,7 @@
         <v>28</v>
       </c>
       <c r="D194" t="str">
-        <v>전정우</v>
+        <v>천명태</v>
       </c>
       <c r="E194" t="str">
         <v>남</v>
@@ -4875,7 +4875,7 @@
         <v>1</v>
       </c>
       <c r="D195" t="str">
-        <v>홍승우</v>
+        <v>성현준</v>
       </c>
       <c r="E195" t="str">
         <v>남</v>
@@ -4898,7 +4898,7 @@
         <v>2</v>
       </c>
       <c r="D196" t="str">
-        <v>김지아</v>
+        <v>윤명주</v>
       </c>
       <c r="E196" t="str">
         <v>남</v>
@@ -4921,7 +4921,7 @@
         <v>3</v>
       </c>
       <c r="D197" t="str">
-        <v>이하윤</v>
+        <v>김태영</v>
       </c>
       <c r="E197" t="str">
         <v>남</v>
@@ -4944,7 +4944,7 @@
         <v>4</v>
       </c>
       <c r="D198" t="str">
-        <v>박서아</v>
+        <v>김민재</v>
       </c>
       <c r="E198" t="str">
         <v>여</v>
@@ -4967,7 +4967,7 @@
         <v>5</v>
       </c>
       <c r="D199" t="str">
-        <v>최아윤</v>
+        <v>정대만</v>
       </c>
       <c r="E199" t="str">
         <v>여</v>
@@ -4990,7 +4990,7 @@
         <v>6</v>
       </c>
       <c r="D200" t="str">
-        <v>정지유</v>
+        <v>김태형</v>
       </c>
       <c r="E200" t="str">
         <v>여</v>
@@ -5013,7 +5013,7 @@
         <v>7</v>
       </c>
       <c r="D201" t="str">
-        <v>강서윤</v>
+        <v>최택</v>
       </c>
       <c r="E201" t="str">
         <v>여</v>
@@ -5036,7 +5036,7 @@
         <v>8</v>
       </c>
       <c r="D202" t="str">
-        <v>조서연</v>
+        <v>써니</v>
       </c>
       <c r="E202" t="str">
         <v>남</v>
@@ -5059,7 +5059,7 @@
         <v>9</v>
       </c>
       <c r="D203" t="str">
-        <v>윤아린</v>
+        <v>지은탁</v>
       </c>
       <c r="E203" t="str">
         <v>여</v>
@@ -5082,7 +5082,7 @@
         <v>10</v>
       </c>
       <c r="D204" t="str">
-        <v>장하은</v>
+        <v>구씨</v>
       </c>
       <c r="E204" t="str">
         <v>남</v>
@@ -5105,7 +5105,7 @@
         <v>11</v>
       </c>
       <c r="D205" t="str">
-        <v>임아은</v>
+        <v>이강인</v>
       </c>
       <c r="E205" t="str">
         <v>여</v>
@@ -5128,7 +5128,7 @@
         <v>12</v>
       </c>
       <c r="D206" t="str">
-        <v>한수아</v>
+        <v>우영우</v>
       </c>
       <c r="E206" t="str">
         <v>여</v>
@@ -5151,7 +5151,7 @@
         <v>13</v>
       </c>
       <c r="D207" t="str">
-        <v>오지우</v>
+        <v>채소연</v>
       </c>
       <c r="E207" t="str">
         <v>여</v>
@@ -5174,7 +5174,7 @@
         <v>14</v>
       </c>
       <c r="D208" t="str">
-        <v>서채원</v>
+        <v>황정민</v>
       </c>
       <c r="E208" t="str">
         <v>남</v>
@@ -5197,7 +5197,7 @@
         <v>15</v>
       </c>
       <c r="D209" t="str">
-        <v>신예린</v>
+        <v>이이</v>
       </c>
       <c r="E209" t="str">
         <v>남</v>
@@ -5220,7 +5220,7 @@
         <v>16</v>
       </c>
       <c r="D210" t="str">
-        <v>권소윤</v>
+        <v>권준호</v>
       </c>
       <c r="E210" t="str">
         <v>남</v>
@@ -5243,7 +5243,7 @@
         <v>17</v>
       </c>
       <c r="D211" t="str">
-        <v>황유나</v>
+        <v>장권혁</v>
       </c>
       <c r="E211" t="str">
         <v>남</v>
@@ -5266,7 +5266,7 @@
         <v>18</v>
       </c>
       <c r="D212" t="str">
-        <v>안지안</v>
+        <v>이황</v>
       </c>
       <c r="E212" t="str">
         <v>여</v>
@@ -5289,7 +5289,7 @@
         <v>19</v>
       </c>
       <c r="D213" t="str">
-        <v>송서율</v>
+        <v>성덕선</v>
       </c>
       <c r="E213" t="str">
         <v>남</v>
@@ -5312,7 +5312,7 @@
         <v>20</v>
       </c>
       <c r="D214" t="str">
-        <v>전시아</v>
+        <v>지석진</v>
       </c>
       <c r="E214" t="str">
         <v>여</v>
@@ -5335,7 +5335,7 @@
         <v>21</v>
       </c>
       <c r="D215" t="str">
-        <v>홍다은</v>
+        <v>신준섭</v>
       </c>
       <c r="E215" t="str">
         <v>남</v>
@@ -5358,7 +5358,7 @@
         <v>22</v>
       </c>
       <c r="D216" t="str">
-        <v>정카라</v>
+        <v>정우성</v>
       </c>
       <c r="E216" t="str">
         <v>남</v>
@@ -5381,7 +5381,7 @@
         <v>23</v>
       </c>
       <c r="D217" t="str">
-        <v>강지지</v>
+        <v>최산해</v>
       </c>
       <c r="E217" t="str">
         <v>여</v>
@@ -5404,7 +5404,7 @@
         <v>24</v>
       </c>
       <c r="D218" t="str">
-        <v>조수시</v>
+        <v>다니엘</v>
       </c>
       <c r="E218" t="str">
         <v>여</v>
@@ -5427,7 +5427,7 @@
         <v>25</v>
       </c>
       <c r="D219" t="str">
-        <v>윤규서</v>
+        <v>김신</v>
       </c>
       <c r="E219" t="str">
         <v>남</v>
@@ -5450,7 +5450,7 @@
         <v>26</v>
       </c>
       <c r="D220" t="str">
-        <v>장자재</v>
+        <v>부승관</v>
       </c>
       <c r="E220" t="str">
         <v>남</v>
@@ -5473,7 +5473,7 @@
         <v>27</v>
       </c>
       <c r="D221" t="str">
-        <v>임현차</v>
+        <v>김승규</v>
       </c>
       <c r="E221" t="str">
         <v>남</v>
@@ -5496,7 +5496,7 @@
         <v>1</v>
       </c>
       <c r="D222" t="str">
-        <v>한호호</v>
+        <v>안기준</v>
       </c>
       <c r="E222" t="str">
         <v>여</v>
@@ -5519,7 +5519,7 @@
         <v>2</v>
       </c>
       <c r="D223" t="str">
-        <v>오연마</v>
+        <v>심청이</v>
       </c>
       <c r="E223" t="str">
         <v>여</v>
@@ -5542,7 +5542,7 @@
         <v>3</v>
       </c>
       <c r="D224" t="str">
-        <v>서바윤</v>
+        <v>최승철</v>
       </c>
       <c r="E224" t="str">
         <v>여</v>
@@ -5565,7 +5565,7 @@
         <v>4</v>
       </c>
       <c r="D225" t="str">
-        <v>신서규</v>
+        <v>은지원</v>
       </c>
       <c r="E225" t="str">
         <v>남</v>
@@ -5588,7 +5588,7 @@
         <v>5</v>
       </c>
       <c r="D226" t="str">
-        <v>권은준</v>
+        <v>차두리</v>
       </c>
       <c r="E226" t="str">
         <v>여</v>
@@ -5611,7 +5611,7 @@
         <v>6</v>
       </c>
       <c r="D227" t="str">
-        <v>황하하</v>
+        <v>염창희</v>
       </c>
       <c r="E227" t="str">
         <v>여</v>
@@ -5634,7 +5634,7 @@
         <v>7</v>
       </c>
       <c r="D228" t="str">
-        <v>안라카</v>
+        <v>정형돈</v>
       </c>
       <c r="E228" t="str">
         <v>여</v>
@@ -5657,7 +5657,7 @@
         <v>8</v>
       </c>
       <c r="D229" t="str">
-        <v>송타영</v>
+        <v>신사임</v>
       </c>
       <c r="E229" t="str">
         <v>남</v>
@@ -5680,7 +5680,7 @@
         <v>9</v>
       </c>
       <c r="D230" t="str">
-        <v>전윤바</v>
+        <v>전정국</v>
       </c>
       <c r="E230" t="str">
         <v>여</v>
@@ -5703,7 +5703,7 @@
         <v>10</v>
       </c>
       <c r="D231" t="str">
-        <v>홍빈아</v>
+        <v>이가은</v>
       </c>
       <c r="E231" t="str">
         <v>여</v>
@@ -5726,7 +5726,7 @@
         <v>11</v>
       </c>
       <c r="D232" t="str">
-        <v>유나나</v>
+        <v>최무선</v>
       </c>
       <c r="E232" t="str">
         <v>여</v>
@@ -5749,7 +5749,7 @@
         <v>12</v>
       </c>
       <c r="D233" t="str">
-        <v>고차현</v>
+        <v>백정태</v>
       </c>
       <c r="E233" t="str">
         <v>남</v>
@@ -5772,7 +5772,7 @@
         <v>13</v>
       </c>
       <c r="D234" t="str">
-        <v>문우도</v>
+        <v>이휘경</v>
       </c>
       <c r="E234" t="str">
         <v>여</v>
@@ -5795,7 +5795,7 @@
         <v>14</v>
       </c>
       <c r="D235" t="str">
-        <v>양영타</v>
+        <v>오청명</v>
       </c>
       <c r="E235" t="str">
         <v>남</v>
@@ -5818,7 +5818,7 @@
         <v>15</v>
       </c>
       <c r="D236" t="str">
-        <v>손시수</v>
+        <v>김종인</v>
       </c>
       <c r="E236" t="str">
         <v>남</v>
@@ -5841,7 +5841,7 @@
         <v>16</v>
       </c>
       <c r="D237" t="str">
-        <v>배사사</v>
+        <v>문태일</v>
       </c>
       <c r="E237" t="str">
         <v>남</v>
@@ -5864,7 +5864,7 @@
         <v>17</v>
       </c>
       <c r="D238" t="str">
-        <v>조준은</v>
+        <v>송혜교</v>
       </c>
       <c r="E238" t="str">
         <v>여</v>
@@ -5887,7 +5887,7 @@
         <v>18</v>
       </c>
       <c r="D239" t="str">
-        <v>백진다</v>
+        <v>유도진</v>
       </c>
       <c r="E239" t="str">
         <v>남</v>
@@ -5910,7 +5910,7 @@
         <v>19</v>
       </c>
       <c r="D240" t="str">
-        <v>허도우</v>
+        <v>김종국</v>
       </c>
       <c r="E240" t="str">
         <v>남</v>
@@ -5933,7 +5933,7 @@
         <v>20</v>
       </c>
       <c r="D241" t="str">
-        <v>남마연</v>
+        <v>이효리</v>
       </c>
       <c r="E241" t="str">
         <v>여</v>
@@ -5956,7 +5956,7 @@
         <v>21</v>
       </c>
       <c r="D242" t="str">
-        <v>김민민</v>
+        <v>김윤석</v>
       </c>
       <c r="E242" t="str">
         <v>남</v>
@@ -5979,7 +5979,7 @@
         <v>22</v>
       </c>
       <c r="D243" t="str">
-        <v>이아빈</v>
+        <v>윤아</v>
       </c>
       <c r="E243" t="str">
         <v>남</v>
@@ -6002,7 +6002,7 @@
         <v>23</v>
       </c>
       <c r="D244" t="str">
-        <v>박재자</v>
+        <v>문현아</v>
       </c>
       <c r="E244" t="str">
         <v>남</v>
@@ -6025,7 +6025,7 @@
         <v>24</v>
       </c>
       <c r="D245" t="str">
-        <v>최다진</v>
+        <v>이훈이</v>
       </c>
       <c r="E245" t="str">
         <v>여</v>
@@ -6048,7 +6048,7 @@
         <v>25</v>
       </c>
       <c r="D246" t="str">
-        <v>정카라</v>
+        <v>박놀부</v>
       </c>
       <c r="E246" t="str">
         <v>남</v>
@@ -6071,7 +6071,7 @@
         <v>26</v>
       </c>
       <c r="D247" t="str">
-        <v>강지지</v>
+        <v>전원우</v>
       </c>
       <c r="E247" t="str">
         <v>여</v>
@@ -6094,7 +6094,7 @@
         <v>27</v>
       </c>
       <c r="D248" t="str">
-        <v>조수시</v>
+        <v>안정원</v>
       </c>
       <c r="E248" t="str">
         <v>남</v>
@@ -6117,7 +6117,7 @@
         <v>28</v>
       </c>
       <c r="D249" t="str">
-        <v>윤규서</v>
+        <v>김광현</v>
       </c>
       <c r="E249" t="str">
         <v>남</v>
@@ -6140,7 +6140,7 @@
         <v>1</v>
       </c>
       <c r="D250" t="str">
-        <v>장자재</v>
+        <v>박지성</v>
       </c>
       <c r="E250" t="str">
         <v>여</v>
@@ -6163,7 +6163,7 @@
         <v>2</v>
       </c>
       <c r="D251" t="str">
-        <v>임현차</v>
+        <v>전소민</v>
       </c>
       <c r="E251" t="str">
         <v>남</v>
@@ -6186,7 +6186,7 @@
         <v>3</v>
       </c>
       <c r="D252" t="str">
-        <v>한호호</v>
+        <v>양호열</v>
       </c>
       <c r="E252" t="str">
         <v>남</v>
@@ -6209,7 +6209,7 @@
         <v>4</v>
       </c>
       <c r="D253" t="str">
-        <v>오연마</v>
+        <v>정도전</v>
       </c>
       <c r="E253" t="str">
         <v>남</v>
@@ -6232,7 +6232,7 @@
         <v>5</v>
       </c>
       <c r="D254" t="str">
-        <v>서바윤</v>
+        <v>아이유</v>
       </c>
       <c r="E254" t="str">
         <v>여</v>
@@ -6255,7 +6255,7 @@
         <v>6</v>
       </c>
       <c r="D255" t="str">
-        <v>신서규</v>
+        <v>안중근</v>
       </c>
       <c r="E255" t="str">
         <v>남</v>
@@ -6278,7 +6278,7 @@
         <v>7</v>
       </c>
       <c r="D256" t="str">
-        <v>권은준</v>
+        <v>김제덕</v>
       </c>
       <c r="E256" t="str">
         <v>여</v>
@@ -6301,7 +6301,7 @@
         <v>8</v>
       </c>
       <c r="D257" t="str">
-        <v>황하하</v>
+        <v>김준면</v>
       </c>
       <c r="E257" t="str">
         <v>남</v>
@@ -6324,7 +6324,7 @@
         <v>9</v>
       </c>
       <c r="D258" t="str">
-        <v>안라카</v>
+        <v>정약용</v>
       </c>
       <c r="E258" t="str">
         <v>여</v>
@@ -6347,7 +6347,7 @@
         <v>10</v>
       </c>
       <c r="D259" t="str">
-        <v>송타영</v>
+        <v>길성준</v>
       </c>
       <c r="E259" t="str">
         <v>남</v>
@@ -6370,7 +6370,7 @@
         <v>11</v>
       </c>
       <c r="D260" t="str">
-        <v>전윤바</v>
+        <v>조규성</v>
       </c>
       <c r="E260" t="str">
         <v>여</v>
@@ -6393,7 +6393,7 @@
         <v>12</v>
       </c>
       <c r="D261" t="str">
-        <v>홍빈아</v>
+        <v>송지효</v>
       </c>
       <c r="E261" t="str">
         <v>남</v>
@@ -6416,7 +6416,7 @@
         <v>13</v>
       </c>
       <c r="D262" t="str">
-        <v>유나나</v>
+        <v>김철수</v>
       </c>
       <c r="E262" t="str">
         <v>여</v>
@@ -6439,7 +6439,7 @@
         <v>14</v>
       </c>
       <c r="D263" t="str">
-        <v>고차현</v>
+        <v>장홍련</v>
       </c>
       <c r="E263" t="str">
         <v>여</v>
@@ -6462,7 +6462,7 @@
         <v>15</v>
       </c>
       <c r="D264" t="str">
-        <v>문우도</v>
+        <v>김남준</v>
       </c>
       <c r="E264" t="str">
         <v>여</v>
@@ -6485,7 +6485,7 @@
         <v>16</v>
       </c>
       <c r="D265" t="str">
-        <v>양영타</v>
+        <v>팜하니</v>
       </c>
       <c r="E265" t="str">
         <v>여</v>
@@ -6508,7 +6508,7 @@
         <v>17</v>
       </c>
       <c r="D266" t="str">
-        <v>손시수</v>
+        <v>윤봉길</v>
       </c>
       <c r="E266" t="str">
         <v>남</v>
@@ -6531,7 +6531,7 @@
         <v>18</v>
       </c>
       <c r="D267" t="str">
-        <v>배사사</v>
+        <v>오창석</v>
       </c>
       <c r="E267" t="str">
         <v>남</v>
@@ -6554,7 +6554,7 @@
         <v>19</v>
       </c>
       <c r="D268" t="str">
-        <v>조준은</v>
+        <v>박찬열</v>
       </c>
       <c r="E268" t="str">
         <v>여</v>
@@ -6577,7 +6577,7 @@
         <v>20</v>
       </c>
       <c r="D269" t="str">
-        <v>백진다</v>
+        <v>최민식</v>
       </c>
       <c r="E269" t="str">
         <v>남</v>
@@ -6600,7 +6600,7 @@
         <v>21</v>
       </c>
       <c r="D270" t="str">
-        <v>허도우</v>
+        <v>매일석</v>
       </c>
       <c r="E270" t="str">
         <v>남</v>
@@ -6623,7 +6623,7 @@
         <v>22</v>
       </c>
       <c r="D271" t="str">
-        <v>남마연</v>
+        <v>남진모</v>
       </c>
       <c r="E271" t="str">
         <v>여</v>
@@ -6646,7 +6646,7 @@
         <v>23</v>
       </c>
       <c r="D272" t="str">
-        <v>김민민</v>
+        <v>홍익현</v>
       </c>
       <c r="E272" t="str">
         <v>남</v>
@@ -6669,7 +6669,7 @@
         <v>24</v>
       </c>
       <c r="D273" t="str">
-        <v>이아빈</v>
+        <v>안정환</v>
       </c>
       <c r="E273" t="str">
         <v>남</v>
@@ -6692,7 +6692,7 @@
         <v>25</v>
       </c>
       <c r="D274" t="str">
-        <v>박재자</v>
+        <v>하도영</v>
       </c>
       <c r="E274" t="str">
         <v>남</v>
@@ -6715,7 +6715,7 @@
         <v>26</v>
       </c>
       <c r="D275" t="str">
-        <v>최다진</v>
+        <v>이순신</v>
       </c>
       <c r="E275" t="str">
         <v>남</v>
@@ -6738,7 +6738,7 @@
         <v>27</v>
       </c>
       <c r="D276" t="str">
-        <v>정카라</v>
+        <v>문준휘</v>
       </c>
       <c r="E276" t="str">
         <v>여</v>
@@ -6761,7 +6761,7 @@
         <v>1</v>
       </c>
       <c r="D277" t="str">
-        <v>강지지</v>
+        <v>김남일</v>
       </c>
       <c r="E277" t="str">
         <v>남</v>
@@ -6784,7 +6784,7 @@
         <v>2</v>
       </c>
       <c r="D278" t="str">
-        <v>조수시</v>
+        <v>채성아</v>
       </c>
       <c r="E278" t="str">
         <v>남</v>
@@ -6807,7 +6807,7 @@
         <v>3</v>
       </c>
       <c r="D279" t="str">
-        <v>윤규서</v>
+        <v>김민석</v>
       </c>
       <c r="E279" t="str">
         <v>남</v>
@@ -6830,7 +6830,7 @@
         <v>4</v>
       </c>
       <c r="D280" t="str">
-        <v>장자재</v>
+        <v>강모연</v>
       </c>
       <c r="E280" t="str">
         <v>남</v>
@@ -6853,7 +6853,7 @@
         <v>5</v>
       </c>
       <c r="D281" t="str">
-        <v>임현차</v>
+        <v>신윤복</v>
       </c>
       <c r="E281" t="str">
         <v>여</v>
@@ -6876,7 +6876,7 @@
         <v>6</v>
       </c>
       <c r="D282" t="str">
-        <v>한호호</v>
+        <v>양석형</v>
       </c>
       <c r="E282" t="str">
         <v>남</v>
@@ -6899,7 +6899,7 @@
         <v>7</v>
       </c>
       <c r="D283" t="str">
-        <v>오연마</v>
+        <v>신나리</v>
       </c>
       <c r="E283" t="str">
         <v>여</v>
@@ -6922,7 +6922,7 @@
         <v>8</v>
       </c>
       <c r="D284" t="str">
-        <v>서바윤</v>
+        <v>손예진</v>
       </c>
       <c r="E284" t="str">
         <v>여</v>
@@ -6945,7 +6945,7 @@
         <v>9</v>
       </c>
       <c r="D285" t="str">
-        <v>신서규</v>
+        <v>변학도</v>
       </c>
       <c r="E285" t="str">
         <v>여</v>
@@ -6968,7 +6968,7 @@
         <v>10</v>
       </c>
       <c r="D286" t="str">
-        <v>권은준</v>
+        <v>박세모</v>
       </c>
       <c r="E286" t="str">
         <v>여</v>
@@ -6991,7 +6991,7 @@
         <v>11</v>
       </c>
       <c r="D287" t="str">
-        <v>황하하</v>
+        <v>황태산</v>
       </c>
       <c r="E287" t="str">
         <v>남</v>
@@ -7014,7 +7014,7 @@
         <v>12</v>
       </c>
       <c r="D288" t="str">
-        <v>안라카</v>
+        <v>송강호</v>
       </c>
       <c r="E288" t="str">
         <v>남</v>
@@ -7037,7 +7037,7 @@
         <v>13</v>
       </c>
       <c r="D289" t="str">
-        <v>송타영</v>
+        <v>이지훈</v>
       </c>
       <c r="E289" t="str">
         <v>남</v>
@@ -7060,7 +7060,7 @@
         <v>14</v>
       </c>
       <c r="D290" t="str">
-        <v>전윤바</v>
+        <v>장영실</v>
       </c>
       <c r="E290" t="str">
         <v>여</v>
@@ -7083,7 +7083,7 @@
         <v>15</v>
       </c>
       <c r="D291" t="str">
-        <v>홍빈아</v>
+        <v>고민구</v>
       </c>
       <c r="E291" t="str">
         <v>여</v>
@@ -7106,7 +7106,7 @@
         <v>16</v>
       </c>
       <c r="D292" t="str">
-        <v>유나나</v>
+        <v>장겨울</v>
       </c>
       <c r="E292" t="str">
         <v>여</v>
@@ -7129,7 +7129,7 @@
         <v>17</v>
       </c>
       <c r="D293" t="str">
-        <v>고차현</v>
+        <v>황희</v>
       </c>
       <c r="E293" t="str">
         <v>여</v>
@@ -7152,7 +7152,7 @@
         <v>18</v>
       </c>
       <c r="D294" t="str">
-        <v>문우도</v>
+        <v>윤성빈</v>
       </c>
       <c r="E294" t="str">
         <v>남</v>
@@ -7175,7 +7175,7 @@
         <v>19</v>
       </c>
       <c r="D295" t="str">
-        <v>양영타</v>
+        <v>을지문</v>
       </c>
       <c r="E295" t="str">
         <v>여</v>
@@ -7198,7 +7198,7 @@
         <v>20</v>
       </c>
       <c r="D296" t="str">
-        <v>손시수</v>
+        <v>이몽룡</v>
       </c>
       <c r="E296" t="str">
         <v>여</v>
@@ -7221,7 +7221,7 @@
         <v>21</v>
       </c>
       <c r="D297" t="str">
-        <v>배사사</v>
+        <v>콩쥐</v>
       </c>
       <c r="E297" t="str">
         <v>남</v>
@@ -7244,7 +7244,7 @@
         <v>22</v>
       </c>
       <c r="D298" t="str">
-        <v>조준은</v>
+        <v>이샤오</v>
       </c>
       <c r="E298" t="str">
         <v>남</v>
@@ -7267,7 +7267,7 @@
         <v>23</v>
       </c>
       <c r="D299" t="str">
-        <v>백진다</v>
+        <v>손흥민</v>
       </c>
       <c r="E299" t="str">
         <v>남</v>
@@ -7290,7 +7290,7 @@
         <v>24</v>
       </c>
       <c r="D300" t="str">
-        <v>허도우</v>
+        <v>김민정</v>
       </c>
       <c r="E300" t="str">
         <v>남</v>
@@ -7313,7 +7313,7 @@
         <v>25</v>
       </c>
       <c r="D301" t="str">
-        <v>남마연</v>
+        <v>이용팔</v>
       </c>
       <c r="E301" t="str">
         <v>여</v>
@@ -7336,7 +7336,7 @@
         <v>26</v>
       </c>
       <c r="D302" t="str">
-        <v>김민민</v>
+        <v>민윤기</v>
       </c>
       <c r="E302" t="str">
         <v>여</v>
@@ -7359,7 +7359,7 @@
         <v>27</v>
       </c>
       <c r="D303" t="str">
-        <v>이아빈</v>
+        <v>염미정</v>
       </c>
       <c r="E303" t="str">
         <v>남</v>
@@ -7382,7 +7382,7 @@
         <v>28</v>
       </c>
       <c r="D304" t="str">
-        <v>박재자</v>
+        <v>김정환</v>
       </c>
       <c r="E304" t="str">
         <v>여</v>
@@ -7405,7 +7405,7 @@
         <v>1</v>
       </c>
       <c r="D305" t="str">
-        <v>최다진</v>
+        <v>이동혁</v>
       </c>
       <c r="E305" t="str">
         <v>여</v>
@@ -7428,7 +7428,7 @@
         <v>2</v>
       </c>
       <c r="D306" t="str">
-        <v>정카라</v>
+        <v>조상우</v>
       </c>
       <c r="E306" t="str">
         <v>남</v>
@@ -7451,7 +7451,7 @@
         <v>3</v>
       </c>
       <c r="D307" t="str">
-        <v>강지지</v>
+        <v>장덕수</v>
       </c>
       <c r="E307" t="str">
         <v>여</v>
@@ -7474,7 +7474,7 @@
         <v>4</v>
       </c>
       <c r="D308" t="str">
-        <v>조수시</v>
+        <v>김석진</v>
       </c>
       <c r="E308" t="str">
         <v>남</v>
@@ -7497,7 +7497,7 @@
         <v>5</v>
       </c>
       <c r="D309" t="str">
-        <v>윤규서</v>
+        <v>도경수</v>
       </c>
       <c r="E309" t="str">
         <v>남</v>
@@ -7520,7 +7520,7 @@
         <v>6</v>
       </c>
       <c r="D310" t="str">
-        <v>장자재</v>
+        <v>류동룡</v>
       </c>
       <c r="E310" t="str">
         <v>남</v>
@@ -7543,7 +7543,7 @@
         <v>7</v>
       </c>
       <c r="D311" t="str">
-        <v>임현차</v>
+        <v>도민준</v>
       </c>
       <c r="E311" t="str">
         <v>여</v>
@@ -7566,7 +7566,7 @@
         <v>8</v>
       </c>
       <c r="D312" t="str">
-        <v>한호호</v>
+        <v>김연아</v>
       </c>
       <c r="E312" t="str">
         <v>여</v>
@@ -7589,7 +7589,7 @@
         <v>9</v>
       </c>
       <c r="D313" t="str">
-        <v>오연마</v>
+        <v>김정우</v>
       </c>
       <c r="E313" t="str">
         <v>남</v>
@@ -7612,7 +7612,7 @@
         <v>10</v>
       </c>
       <c r="D314" t="str">
-        <v>서바윤</v>
+        <v>이수근</v>
       </c>
       <c r="E314" t="str">
         <v>남</v>
@@ -7635,7 +7635,7 @@
         <v>11</v>
       </c>
       <c r="D315" t="str">
-        <v>신서규</v>
+        <v>김종대</v>
       </c>
       <c r="E315" t="str">
         <v>남</v>
@@ -7658,7 +7658,7 @@
         <v>12</v>
       </c>
       <c r="D316" t="str">
-        <v>권은준</v>
+        <v>유아인</v>
       </c>
       <c r="E316" t="str">
         <v>남</v>
@@ -7681,7 +7681,7 @@
         <v>13</v>
       </c>
       <c r="D317" t="str">
-        <v>황하하</v>
+        <v>또치</v>
       </c>
       <c r="E317" t="str">
         <v>남</v>
@@ -7704,7 +7704,7 @@
         <v>14</v>
       </c>
       <c r="D318" t="str">
-        <v>안라카</v>
+        <v>박서준</v>
       </c>
       <c r="E318" t="str">
         <v>여</v>
@@ -7727,7 +7727,7 @@
         <v>15</v>
       </c>
       <c r="D319" t="str">
-        <v>송타영</v>
+        <v>고뭉치</v>
       </c>
       <c r="E319" t="str">
         <v>남</v>
@@ -7750,7 +7750,7 @@
         <v>16</v>
       </c>
       <c r="D320" t="str">
-        <v>전윤바</v>
+        <v>이한나</v>
       </c>
       <c r="E320" t="str">
         <v>여</v>
@@ -7773,7 +7773,7 @@
         <v>17</v>
       </c>
       <c r="D321" t="str">
-        <v>홍빈아</v>
+        <v>이재성</v>
       </c>
       <c r="E321" t="str">
         <v>여</v>
@@ -7796,7 +7796,7 @@
         <v>18</v>
       </c>
       <c r="D322" t="str">
-        <v>유나나</v>
+        <v>장한솔</v>
       </c>
       <c r="E322" t="str">
         <v>여</v>
@@ -7819,7 +7819,7 @@
         <v>19</v>
       </c>
       <c r="D323" t="str">
-        <v>고차현</v>
+        <v>정몽주</v>
       </c>
       <c r="E323" t="str">
         <v>여</v>
@@ -7842,7 +7842,7 @@
         <v>20</v>
       </c>
       <c r="D324" t="str">
-        <v>문우도</v>
+        <v>권지옹</v>
       </c>
       <c r="E324" t="str">
         <v>여</v>
@@ -7865,7 +7865,7 @@
         <v>21</v>
       </c>
       <c r="D325" t="str">
-        <v>양영타</v>
+        <v>이상화</v>
       </c>
       <c r="E325" t="str">
         <v>남</v>
@@ -7888,7 +7888,7 @@
         <v>22</v>
       </c>
       <c r="D326" t="str">
-        <v>손시수</v>
+        <v>장원영</v>
       </c>
       <c r="E326" t="str">
         <v>남</v>
@@ -7911,7 +7911,7 @@
         <v>23</v>
       </c>
       <c r="D327" t="str">
-        <v>배사사</v>
+        <v>김연경</v>
       </c>
       <c r="E327" t="str">
         <v>여</v>
@@ -7934,7 +7934,7 @@
         <v>24</v>
       </c>
       <c r="D328" t="str">
-        <v>조준은</v>
+        <v>이제노</v>
       </c>
       <c r="E328" t="str">
         <v>남</v>
@@ -7957,7 +7957,7 @@
         <v>25</v>
       </c>
       <c r="D329" t="str">
-        <v>백진다</v>
+        <v>박태환</v>
       </c>
       <c r="E329" t="str">
         <v>남</v>
@@ -7980,7 +7980,7 @@
         <v>26</v>
       </c>
       <c r="D330" t="str">
-        <v>허도우</v>
+        <v>채송화</v>
       </c>
       <c r="E330" t="str">
         <v>여</v>
@@ -8003,7 +8003,7 @@
         <v>27</v>
       </c>
       <c r="D331" t="str">
-        <v>남마연</v>
+        <v>이익준</v>
       </c>
       <c r="E331" t="str">
         <v>남</v>

</xml_diff>